<commit_message>
Changes to table and model
Changed the model code and weights in table for manuscript
</commit_message>
<xml_diff>
--- a/Data/Table S1 lakes and attributes.xlsx
+++ b/Data/Table S1 lakes and attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylel\OneDrive\Documents\GitHub\anglers-lakers\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534DEFAA-41A1-4265-A265-16A318F81B26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88A39A-A873-4A64-AD74-A268143C6AFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1" xr2:uid="{3803C25B-C301-4489-9798-1F4D38B7938A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3803C25B-C301-4489-9798-1F4D38B7938A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2616,7 +2616,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,7 +2745,7 @@
         <v>66455</v>
       </c>
       <c r="N3" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O3">
         <v>140</v>
@@ -2792,7 +2792,7 @@
         <v>242766</v>
       </c>
       <c r="N4" s="8">
-        <v>0.86440677966101698</v>
+        <v>0.33</v>
       </c>
       <c r="O4">
         <v>144</v>
@@ -2839,7 +2839,7 @@
         <v>28629</v>
       </c>
       <c r="N5" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.13</v>
       </c>
       <c r="O5">
         <v>23</v>
@@ -2886,7 +2886,7 @@
         <v>50590</v>
       </c>
       <c r="N6" s="8">
-        <v>0.86440677966101698</v>
+        <v>0.33</v>
       </c>
       <c r="O6">
         <v>67</v>
@@ -2933,7 +2933,7 @@
         <v>9102</v>
       </c>
       <c r="N7" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O7">
         <v>49</v>
@@ -2980,7 +2980,7 @@
         <v>41787</v>
       </c>
       <c r="N8" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.13</v>
       </c>
       <c r="O8">
         <v>74</v>
@@ -3027,7 +3027,7 @@
         <v>75562</v>
       </c>
       <c r="N9" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.22</v>
       </c>
       <c r="O9">
         <v>46</v>
@@ -3074,7 +3074,7 @@
         <v>5397</v>
       </c>
       <c r="N10" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.22</v>
       </c>
       <c r="O10">
         <v>95</v>
@@ -3121,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="N11" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O11">
         <v>54</v>
@@ -3168,7 +3168,7 @@
         <v>2874</v>
       </c>
       <c r="N12" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O12">
         <v>42</v>
@@ -3215,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="N13" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O13">
         <v>46</v>
@@ -3262,7 +3262,7 @@
         <v>78045</v>
       </c>
       <c r="N14" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.22</v>
       </c>
       <c r="O14">
         <v>192</v>
@@ -3309,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="N15" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.22</v>
       </c>
       <c r="O15">
         <v>63</v>
@@ -3356,7 +3356,7 @@
         <v>51926</v>
       </c>
       <c r="N16" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.22</v>
       </c>
       <c r="O16">
         <v>111</v>
@@ -3403,7 +3403,7 @@
         <v>7178</v>
       </c>
       <c r="N17" s="8">
-        <v>0.23050847457627099</v>
+        <v>0.13</v>
       </c>
       <c r="O17">
         <v>47</v>
@@ -3450,7 +3450,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="8">
-        <v>0.23050847457627099</v>
+        <v>0.13</v>
       </c>
       <c r="O18">
         <v>56</v>
@@ -3497,7 +3497,7 @@
         <v>9976</v>
       </c>
       <c r="N19" s="8">
-        <v>1.23486682808717</v>
+        <v>5.01</v>
       </c>
       <c r="O19">
         <v>64</v>
@@ -3544,7 +3544,7 @@
         <v>17392</v>
       </c>
       <c r="N20" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.13</v>
       </c>
       <c r="O20">
         <v>94</v>
@@ -3591,7 +3591,7 @@
         <v>2</v>
       </c>
       <c r="N21" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.13</v>
       </c>
       <c r="O21">
         <v>87</v>
@@ -3638,7 +3638,7 @@
         <v>2</v>
       </c>
       <c r="N22" s="8">
-        <v>2.0169491525423702</v>
+        <v>0.27</v>
       </c>
       <c r="O22">
         <v>164</v>
@@ -3685,7 +3685,7 @@
         <v>764</v>
       </c>
       <c r="N23" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O23">
         <v>24</v>
@@ -3732,7 +3732,7 @@
         <v>17865</v>
       </c>
       <c r="N24" s="8">
-        <v>1.23486682808717</v>
+        <v>0.33</v>
       </c>
       <c r="O24">
         <v>26</v>
@@ -3779,7 +3779,7 @@
         <v>2</v>
       </c>
       <c r="N25" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O25">
         <v>17</v>
@@ -3826,7 +3826,7 @@
         <v>2</v>
       </c>
       <c r="N26" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O26">
         <v>5</v>
@@ -3873,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="N27" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O27">
         <v>8</v>
@@ -3920,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="N28" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O28">
         <v>2</v>
@@ -3967,7 +3967,7 @@
         <v>162460</v>
       </c>
       <c r="N29" s="8">
-        <v>0.51864406779660999</v>
+        <v>0.13</v>
       </c>
       <c r="O29">
         <v>223</v>
@@ -4014,7 +4014,7 @@
         <v>680</v>
       </c>
       <c r="N30" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -4061,7 +4061,7 @@
         <v>2</v>
       </c>
       <c r="N31" s="8">
-        <v>2.0169491525423702</v>
+        <v>1.53</v>
       </c>
       <c r="O31">
         <v>33</v>
@@ -4108,7 +4108,7 @@
         <v>2</v>
       </c>
       <c r="N32" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O32">
         <v>46</v>
@@ -4155,7 +4155,7 @@
         <v>67603</v>
       </c>
       <c r="N33" s="8">
-        <v>0.23050847457627099</v>
+        <v>0.13</v>
       </c>
       <c r="O33">
         <v>81</v>
@@ -4202,7 +4202,7 @@
         <v>2</v>
       </c>
       <c r="N34" s="8">
-        <v>0.23050847457627099</v>
+        <v>0.13</v>
       </c>
       <c r="O34">
         <v>22</v>
@@ -4249,7 +4249,7 @@
         <v>2</v>
       </c>
       <c r="N35" s="8">
-        <v>0.23050847457627099</v>
+        <v>0.13</v>
       </c>
       <c r="O35">
         <v>63</v>
@@ -4296,7 +4296,7 @@
         <v>234</v>
       </c>
       <c r="N36" s="8">
-        <v>0.72033898305084698</v>
+        <v>0.27</v>
       </c>
       <c r="O36">
         <v>22</v>
@@ -4304,7 +4304,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:O36" xr:uid="{E4562142-CBC2-4751-B81F-E8A1E45F3F76}">
-    <sortState ref="A3:O36">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O36">
       <sortCondition ref="A2:A36"/>
     </sortState>
   </autoFilter>

</xml_diff>